<commit_message>
ivf, doulas, assisted suicide
</commit_message>
<xml_diff>
--- a/docs/ValueSet-ConsentExchangePolicies.xlsx
+++ b/docs/ValueSet-ConsentExchangePolicies.xlsx
@@ -46,7 +46,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -55,7 +55,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-10-31T09:00:56-05:00</t>
+    <t>2023-11-18T22:49:36-06:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>